<commit_message>
Updated renewables and battery capital and operating costs to 2024 ATB and 2022 USD
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/ereznic2_nrel_gov/Documents/Documents/Projects/Wind-H2-Steel/Modeling/GreenSteel/src/ereznic2/H2_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C39CE12-8F76-461B-8B70-4D91A33E514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{7C39CE12-8F76-461B-8B70-4D91A33E514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB1A9B2D-A398-450D-8A1D-39024D2A9849}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1620" windowWidth="12825" windowHeight="18870" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="-17388" yWindow="-4752" windowWidth="17496" windowHeight="30936" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,8 +178,17 @@
     <t>Iron Ore Pellets Transport ($/metric tonne)</t>
   </si>
   <si>
+    <t>42.4, -90.85</t>
+  </si>
+  <si>
+    <t>29.92, -100.647</t>
+  </si>
+  <si>
+    <t>47.5, -93.00</t>
+  </si>
+  <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -193,7 +202,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -207,7 +216,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -221,7 +230,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -232,15 +241,6 @@
       </rPr>
       <t xml:space="preserve"> PV OpEx</t>
     </r>
-  </si>
-  <si>
-    <t>42.4, -90.85</t>
-  </si>
-  <si>
-    <t>29.92, -100.647</t>
-  </si>
-  <si>
-    <t>47.5, -93.00</t>
   </si>
 </sst>
 </file>
@@ -640,19 +640,19 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="F28" sqref="F28:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -700,19 +700,19 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -732,7 +732,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -752,7 +752,7 @@
         <v>-93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -772,7 +772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -792,7 +792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -812,107 +812,107 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4">
-        <v>1302</v>
+        <v>1666</v>
       </c>
       <c r="C9" s="4">
-        <v>1302</v>
+        <v>1666</v>
       </c>
       <c r="D9" s="6">
-        <v>1422</v>
+        <v>1803</v>
       </c>
       <c r="E9" s="4">
-        <v>1873</v>
+        <v>2335</v>
       </c>
       <c r="F9" s="4">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4">
-        <v>1211</v>
+        <v>1569</v>
       </c>
       <c r="C10" s="4">
-        <v>1211</v>
+        <v>1569</v>
       </c>
       <c r="D10" s="6">
-        <v>1301</v>
+        <v>1703</v>
       </c>
       <c r="E10" s="4">
-        <v>1692</v>
+        <v>2151</v>
       </c>
       <c r="F10" s="4">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4">
-        <v>1098</v>
+        <v>1408</v>
       </c>
       <c r="C11" s="4">
-        <v>1098</v>
+        <v>1408</v>
       </c>
       <c r="D11" s="1">
-        <v>1150</v>
+        <v>1537</v>
       </c>
       <c r="E11" s="4">
-        <v>1467</v>
+        <v>1844</v>
       </c>
       <c r="F11" s="4">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4">
-        <v>1044</v>
+        <v>1335</v>
       </c>
       <c r="C12" s="4">
-        <v>1044</v>
+        <v>1335</v>
       </c>
       <c r="D12" s="1">
-        <v>1093</v>
+        <v>1457</v>
       </c>
       <c r="E12" s="4">
-        <v>1396</v>
+        <v>1749</v>
       </c>
       <c r="F12" s="4">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="4">
-        <v>882</v>
+        <v>1115</v>
       </c>
       <c r="C13" s="4">
-        <v>882</v>
+        <v>1115</v>
       </c>
       <c r="D13" s="1">
-        <v>924</v>
+        <v>1219</v>
       </c>
       <c r="E13" s="4">
-        <v>1185</v>
+        <v>1463</v>
       </c>
       <c r="F13" s="4">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -932,107 +932,107 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4">
-        <v>28.9</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4">
-        <v>28.9</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1">
-        <v>27.2</v>
+        <v>30</v>
       </c>
       <c r="E15" s="4">
-        <v>28.9</v>
+        <v>32</v>
       </c>
       <c r="F15" s="4">
-        <v>28.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="4">
-        <v>27.5</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4">
-        <v>27.5</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1">
-        <v>25.6</v>
+        <v>29</v>
       </c>
       <c r="E16" s="4">
-        <v>27.5</v>
+        <v>31</v>
       </c>
       <c r="F16" s="4">
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="4">
-        <v>25.8</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4">
-        <v>25.8</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1">
-        <v>23.5</v>
+        <v>27</v>
       </c>
       <c r="E17" s="4">
-        <v>25.8</v>
+        <v>29</v>
       </c>
       <c r="F17" s="4">
-        <v>25.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="4">
-        <v>24.9</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4">
-        <v>24.9</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1">
-        <v>22.7</v>
+        <v>26</v>
       </c>
       <c r="E18" s="4">
-        <v>24.9</v>
+        <v>28</v>
       </c>
       <c r="F18" s="4">
-        <v>24.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="4">
-        <v>22.3</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4">
-        <v>22.3</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1">
-        <v>20.3</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4">
-        <v>22.3</v>
+        <v>25</v>
       </c>
       <c r="F19" s="4">
-        <v>22.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1060,107 +1060,107 @@
       <c r="E21" s="1"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4">
-        <v>1233</v>
+        <v>1483</v>
       </c>
       <c r="C22" s="4">
-        <v>1233</v>
+        <v>1483</v>
       </c>
       <c r="D22" s="4">
-        <v>1233</v>
+        <v>1483</v>
       </c>
       <c r="E22" s="4">
-        <v>1233</v>
+        <v>1483</v>
       </c>
       <c r="F22" s="4">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="4">
-        <v>1192</v>
+        <v>1492</v>
       </c>
       <c r="C23" s="4">
-        <v>1192</v>
+        <v>1492</v>
       </c>
       <c r="D23" s="4">
-        <v>1192</v>
+        <v>1492</v>
       </c>
       <c r="E23" s="4">
-        <v>1192</v>
+        <v>1492</v>
       </c>
       <c r="F23" s="4">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="4">
-        <v>991</v>
+        <v>1193</v>
       </c>
       <c r="C24" s="4">
-        <v>991</v>
+        <v>1193</v>
       </c>
       <c r="D24" s="4">
-        <v>991</v>
+        <v>1193</v>
       </c>
       <c r="E24" s="4">
-        <v>991</v>
+        <v>1193</v>
       </c>
       <c r="F24" s="4">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="4">
-        <v>792</v>
+        <v>895</v>
       </c>
       <c r="C25" s="4">
-        <v>792</v>
+        <v>895</v>
       </c>
       <c r="D25" s="4">
-        <v>792</v>
+        <v>895</v>
       </c>
       <c r="E25" s="4">
-        <v>792</v>
+        <v>895</v>
       </c>
       <c r="F25" s="4">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="4">
-        <v>604</v>
+        <v>683</v>
       </c>
       <c r="C26" s="4">
-        <v>604</v>
+        <v>683</v>
       </c>
       <c r="D26" s="4">
-        <v>604</v>
+        <v>683</v>
       </c>
       <c r="E26" s="4">
-        <v>604</v>
+        <v>683</v>
       </c>
       <c r="F26" s="4">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1180,107 +1180,107 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4">
-        <v>21.5</v>
+        <v>24</v>
       </c>
       <c r="C28" s="4">
-        <v>21.5</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4">
-        <v>21.5</v>
+        <v>24</v>
       </c>
       <c r="E28" s="4">
-        <v>21.5</v>
+        <v>24</v>
       </c>
       <c r="F28" s="4">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="4">
-        <v>19.600000000000001</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4">
-        <v>19.600000000000001</v>
+        <v>21</v>
       </c>
       <c r="D29" s="4">
-        <v>19.600000000000001</v>
+        <v>21</v>
       </c>
       <c r="E29" s="4">
-        <v>19.600000000000001</v>
+        <v>21</v>
       </c>
       <c r="F29" s="4">
-        <v>19.600000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4">
-        <v>17.2</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4">
-        <v>17.2</v>
+        <v>18</v>
       </c>
       <c r="D30" s="4">
-        <v>17.2</v>
+        <v>18</v>
       </c>
       <c r="E30" s="4">
-        <v>17.2</v>
+        <v>18</v>
       </c>
       <c r="F30" s="4">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="4">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="C31" s="4">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="D31" s="4">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="E31" s="4">
-        <v>14.8</v>
+        <v>15</v>
       </c>
       <c r="F31" s="4">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B32" s="4">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="C32" s="4">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="D32" s="4">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="E32" s="4">
-        <v>12.9</v>
+        <v>13</v>
       </c>
       <c r="F32" s="4">
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1308,7 +1308,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>46.97</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1439,7 +1439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1451,7 +1451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated natural gas price csv files and steel feedstock costs to 2022 USD
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/ereznic2_nrel_gov/Documents/Documents/Projects/Wind-H2-Steel/Modeling/GreenSteel/src/ereznic2/H2_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{7C39CE12-8F76-461B-8B70-4D91A33E514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB1A9B2D-A398-450D-8A1D-39024D2A9849}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D28933D-33BC-497C-9210-14828DC17EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-4752" windowWidth="17496" windowHeight="30936" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="18645" yWindow="1185" windowWidth="18060" windowHeight="19770" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -247,6 +247,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,6 +324,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -640,19 +649,19 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F32"/>
+      <selection activeCell="B35" sqref="B35:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -692,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -712,7 +721,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -732,7 +741,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -752,7 +761,7 @@
         <v>-93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -772,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -792,7 +801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -812,7 +821,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>49</v>
       </c>
@@ -832,7 +841,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -852,7 +861,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -872,7 +881,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -892,7 +901,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -912,7 +921,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -932,7 +941,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -952,7 +961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -972,7 +981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1032,7 +1041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1060,7 +1069,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1100,7 +1109,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +1169,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1180,7 +1189,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
@@ -1200,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -1220,7 +1229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1300,7 +1309,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1308,124 +1317,124 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="1">
-        <v>100</v>
-      </c>
-      <c r="C35" s="1">
-        <v>100</v>
-      </c>
-      <c r="D35" s="1">
-        <v>100</v>
-      </c>
-      <c r="E35" s="1">
-        <v>100</v>
-      </c>
-      <c r="F35" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="8">
+        <v>108.00738007380073</v>
+      </c>
+      <c r="C35" s="8">
+        <v>108.00738007380073</v>
+      </c>
+      <c r="D35" s="8">
+        <v>108.00738007380073</v>
+      </c>
+      <c r="E35" s="8">
+        <v>108.00738007380073</v>
+      </c>
+      <c r="F35" s="8">
+        <v>108.00738007380073</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="1">
-        <v>190</v>
-      </c>
-      <c r="C36" s="1">
-        <v>190</v>
-      </c>
-      <c r="D36" s="1">
-        <v>190</v>
-      </c>
-      <c r="E36" s="1">
-        <v>190</v>
-      </c>
-      <c r="F36" s="1">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="8">
+        <v>205.2140221402214</v>
+      </c>
+      <c r="C36" s="8">
+        <v>205.2140221402214</v>
+      </c>
+      <c r="D36" s="8">
+        <v>205.2140221402214</v>
+      </c>
+      <c r="E36" s="8">
+        <v>205.2140221402214</v>
+      </c>
+      <c r="F36" s="8">
+        <v>205.2140221402214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="1">
-        <v>207</v>
-      </c>
-      <c r="C37" s="1">
-        <v>207</v>
-      </c>
-      <c r="D37" s="1">
-        <v>207</v>
-      </c>
-      <c r="E37" s="1">
-        <v>207</v>
-      </c>
-      <c r="F37" s="1">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="8">
+        <v>223.57527675276751</v>
+      </c>
+      <c r="C37" s="8">
+        <v>223.57527675276751</v>
+      </c>
+      <c r="D37" s="8">
+        <v>223.57527675276751</v>
+      </c>
+      <c r="E37" s="8">
+        <v>223.57527675276751</v>
+      </c>
+      <c r="F37" s="8">
+        <v>223.57527675276751</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="1">
-        <v>15.3</v>
-      </c>
-      <c r="C38" s="1">
-        <v>74.010000000000005</v>
-      </c>
-      <c r="D38" s="1">
-        <v>15.68</v>
-      </c>
-      <c r="E38" s="1">
-        <v>24.28</v>
-      </c>
-      <c r="F38" s="1">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="7">
+        <v>20.23</v>
+      </c>
+      <c r="C38" s="7">
+        <v>23.91</v>
+      </c>
+      <c r="D38" s="7">
+        <v>43.69</v>
+      </c>
+      <c r="E38" s="7">
+        <v>29.3</v>
+      </c>
+      <c r="F38" s="7">
+        <v>47.72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="1">
-        <v>27.89</v>
-      </c>
-      <c r="C39" s="1">
-        <v>99.45</v>
-      </c>
-      <c r="D39" s="1">
-        <v>18.71</v>
-      </c>
-      <c r="E39" s="1">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="F39" s="1">
-        <v>46.97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="7">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="C39" s="7">
+        <v>75.97</v>
+      </c>
+      <c r="D39" s="7">
+        <v>58.29</v>
+      </c>
+      <c r="E39" s="7">
+        <v>22.92</v>
+      </c>
+      <c r="F39" s="7">
+        <v>64.91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="1">
-        <v>14.52</v>
-      </c>
-      <c r="C40" s="1">
-        <v>133.47</v>
-      </c>
-      <c r="D40" s="1">
-        <v>17.739999999999998</v>
-      </c>
-      <c r="E40" s="1">
-        <v>57.59</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0.35</v>
+      <c r="B40" s="7">
+        <v>23.91</v>
+      </c>
+      <c r="C40" s="7">
+        <v>92.59</v>
+      </c>
+      <c r="D40" s="7">
+        <v>49.85</v>
+      </c>
+      <c r="E40" s="7">
+        <v>65.37</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.63</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1448,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1451,7 +1460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Texas location and grid interconnection costs
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evan\Documents\Work\Green steel\Modeling\GreenSteel\src\ereznic2\H2_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereznic2\Documents\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D28933D-33BC-497C-9210-14828DC17EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72C72A9-E18C-40EF-BBBB-331E43E5E002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18645" yWindow="1185" windowWidth="18060" windowHeight="19770" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="1752" yWindow="1104" windowWidth="19680" windowHeight="15324" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -181,14 +181,11 @@
     <t>42.4, -90.85</t>
   </si>
   <si>
-    <t>29.92, -100.647</t>
-  </si>
-  <si>
     <t>47.5, -93.00</t>
   </si>
   <si>
     <r>
-      <t>2022</t>
+      <t>2020</t>
     </r>
     <r>
       <rPr>
@@ -202,7 +199,7 @@
   </si>
   <si>
     <r>
-      <t>2022</t>
+      <t>2020</t>
     </r>
     <r>
       <rPr>
@@ -216,7 +213,7 @@
   </si>
   <si>
     <r>
-      <t>2022</t>
+      <t>2020</t>
     </r>
     <r>
       <rPr>
@@ -230,7 +227,7 @@
   </si>
   <si>
     <r>
-      <t>2022</t>
+      <t>2020</t>
     </r>
     <r>
       <rPr>
@@ -242,13 +239,16 @@
       <t xml:space="preserve"> PV OpEx</t>
     </r>
   </si>
+  <si>
+    <t>32.318714, -100.18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -329,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,19 +649,19 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:F37"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -709,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>46</v>
@@ -718,18 +718,18 @@
         <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>41.62</v>
       </c>
-      <c r="C4" s="1">
-        <v>29.92</v>
+      <c r="C4" s="7">
+        <v>32.318714</v>
       </c>
       <c r="D4" s="1">
         <v>42.4</v>
@@ -741,7 +741,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -749,7 +749,7 @@
         <v>-87.22</v>
       </c>
       <c r="C5" s="1">
-        <v>-100.64700000000001</v>
+        <v>-100.18</v>
       </c>
       <c r="D5" s="1">
         <v>-90.85</v>
@@ -761,7 +761,7 @@
         <v>-93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -781,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -801,7 +801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -821,9 +821,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4">
         <v>1666</v>
@@ -841,7 +841,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -861,7 +861,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -881,7 +881,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -901,7 +901,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -921,7 +921,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -941,9 +941,9 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4">
         <v>32</v>
@@ -961,7 +961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -981,7 +981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1069,9 +1069,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4">
         <v>1483</v>
@@ -1089,7 +1089,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1189,9 +1189,9 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4">
         <v>24</v>
@@ -1209,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1317,7 +1317,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>108.00738007380073</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>205.2140221402214</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1377,64 +1377,64 @@
         <v>223.57527675276751</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="7">
-        <v>20.23</v>
+        <v>20.91</v>
       </c>
       <c r="C38" s="7">
-        <v>23.91</v>
+        <v>25.87</v>
       </c>
       <c r="D38" s="7">
-        <v>43.69</v>
+        <v>47.26</v>
       </c>
       <c r="E38" s="7">
-        <v>29.3</v>
+        <v>30.91</v>
       </c>
       <c r="F38" s="7">
-        <v>47.72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>49.34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="7">
-        <v>32.340000000000003</v>
+        <v>33.340000000000003</v>
       </c>
       <c r="C39" s="7">
-        <v>75.97</v>
+        <v>79.680000000000007</v>
       </c>
       <c r="D39" s="7">
-        <v>58.29</v>
+        <v>61.68</v>
       </c>
       <c r="E39" s="7">
-        <v>22.92</v>
+        <v>23.72</v>
       </c>
       <c r="F39" s="7">
-        <v>64.91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67.430000000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="7">
-        <v>23.91</v>
+        <v>24.04</v>
       </c>
       <c r="C40" s="7">
-        <v>92.59</v>
+        <v>95.83</v>
       </c>
       <c r="D40" s="7">
-        <v>49.85</v>
+        <v>52.38</v>
       </c>
       <c r="E40" s="7">
-        <v>65.37</v>
+        <v>65.7</v>
       </c>
       <c r="F40" s="7">
-        <v>0.63</v>
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>
@@ -1448,7 +1448,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1460,7 +1460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enabled model to run with 2022 technology costs
</commit_message>
<xml_diff>
--- a/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
+++ b/src/ereznic2/H2_Analysis/green_steel_site_renewable_costs_ATB_aug2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ereznic2\Documents\GreenSteel\src\ereznic2\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72C72A9-E18C-40EF-BBBB-331E43E5E002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8E16F2-53EF-430E-ACB6-2097C8796D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="1104" windowWidth="19680" windowHeight="15324" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
+    <workbookView xWindow="3456" yWindow="2772" windowWidth="15396" windowHeight="14508" xr2:uid="{6F370ACC-2FEA-4034-9DAD-6260C657696D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,8 +184,11 @@
     <t>47.5, -93.00</t>
   </si>
   <si>
+    <t>32.318714, -100.18</t>
+  </si>
+  <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -199,7 +202,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -213,7 +216,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -227,7 +230,7 @@
   </si>
   <si>
     <r>
-      <t>2020</t>
+      <t>2022</t>
     </r>
     <r>
       <rPr>
@@ -238,9 +241,6 @@
       </rPr>
       <t xml:space="preserve"> PV OpEx</t>
     </r>
-  </si>
-  <si>
-    <t>32.318714, -100.18</t>
   </si>
 </sst>
 </file>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F89DB1-4222-400F-9657-1F6A62D7140D}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>46</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="4">
         <v>1666</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4">
         <v>32</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4">
         <v>1483</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>24</v>

</xml_diff>